<commit_message>
Update ATmega48A-PA-88A-PA-168A-PA-328-P-DS-DS40002061A.pdf, MAC8M.pdf, and 6 more files...
</commit_message>
<xml_diff>
--- a/electronics/worksheets/Open-Boiler.xlsx
+++ b/electronics/worksheets/Open-Boiler.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gcasanova\Source\Repos\GitHub\open-boiler\electronics\worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\casanovg\Desktop\open-boiler-testbed\electronics\worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F7A0A5-30E4-4808-AE3D-6E68798B6EFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49B1E74-9C42-4B83-82E7-2A52B8F82CA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3705" yWindow="1500" windowWidth="20880" windowHeight="13410" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T7335D Datasheet" sheetId="4" r:id="rId1"/>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="101">
   <si>
     <t xml:space="preserve"> NTC thermistor table</t>
   </si>
@@ -533,7 +533,7 @@
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -643,14 +643,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1062,7 +1054,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="182">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1346,6 +1338,14 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1367,23 +1367,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="3" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="3" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="166" fontId="3" fillId="16" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1567,7 +1556,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1692,7 +1681,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-AR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1953,7 +1942,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1991,7 +1980,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="946760864"/>
@@ -2098,7 +2087,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2136,7 +2125,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="950936336"/>
@@ -2169,7 +2158,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-AR"/>
               </a:p>
             </c:txPr>
           </c:dispUnitsLbl>
@@ -2209,7 +2198,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2285,7 +2274,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2365,7 +2354,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-AR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -2577,7 +2566,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2615,7 +2604,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="946760864"/>
@@ -2684,7 +2673,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-AR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2722,7 +2711,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="950936336"/>
@@ -2763,7 +2752,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4543,14 +4532,14 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="167" t="s">
+      <c r="B4" s="171" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="168"/>
-      <c r="D4" s="167" t="s">
+      <c r="C4" s="172"/>
+      <c r="D4" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="168"/>
+      <c r="E4" s="172"/>
       <c r="G4" s="18" t="str">
         <f>B4</f>
         <v>Temperature</v>
@@ -6262,14 +6251,14 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="169" t="s">
+      <c r="B4" s="173" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="170"/>
-      <c r="D4" s="169" t="s">
+      <c r="C4" s="174"/>
+      <c r="D4" s="173" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="170"/>
+      <c r="E4" s="174"/>
       <c r="G4" s="22" t="str">
         <f>B4</f>
         <v>Temperature</v>
@@ -6701,10 +6690,10 @@
       <c r="E21" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G21" s="171" t="s">
+      <c r="G21" s="175" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="172"/>
+      <c r="H21" s="176"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
@@ -7062,7 +7051,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B29436D-DFE2-4DAF-A0BC-2A553066C113}">
   <dimension ref="B2:X148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="R87" sqref="R87"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8876,7 +8867,7 @@
         <f t="shared" si="6"/>
         <v>-2.8205128205128216E-2</v>
       </c>
-      <c r="P61" s="173" t="s">
+      <c r="P61" s="177" t="s">
         <v>32</v>
       </c>
     </row>
@@ -8900,7 +8891,7 @@
         <f t="shared" si="6"/>
         <v>-2.6385224274406371E-2</v>
       </c>
-      <c r="P62" s="173"/>
+      <c r="P62" s="177"/>
     </row>
     <row r="63" spans="7:16" x14ac:dyDescent="0.25">
       <c r="J63" s="84">
@@ -8923,7 +8914,7 @@
         <f t="shared" si="6"/>
         <v>-2.7100271002710064E-2</v>
       </c>
-      <c r="P63" s="173"/>
+      <c r="P63" s="177"/>
     </row>
     <row r="64" spans="7:16" x14ac:dyDescent="0.25">
       <c r="J64" s="97">
@@ -8945,7 +8936,7 @@
         <f t="shared" si="6"/>
         <v>-2.2284122562674091E-2</v>
       </c>
-      <c r="P64" s="173"/>
+      <c r="P64" s="177"/>
     </row>
     <row r="65" spans="7:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J65" s="97">
@@ -8967,7 +8958,7 @@
         <f t="shared" si="6"/>
         <v>-2.5641025641025661E-2</v>
       </c>
-      <c r="P65" s="173"/>
+      <c r="P65" s="177"/>
     </row>
     <row r="66" spans="7:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J66" s="97">
@@ -8989,7 +8980,7 @@
         <f t="shared" si="6"/>
         <v>-2.3391812865497075E-2</v>
       </c>
-      <c r="P66" s="173"/>
+      <c r="P66" s="177"/>
     </row>
     <row r="67" spans="7:24" x14ac:dyDescent="0.25">
       <c r="J67" s="97">
@@ -9011,7 +9002,7 @@
         <f t="shared" si="6"/>
         <v>-2.6946107784431184E-2</v>
       </c>
-      <c r="P67" s="173"/>
+      <c r="P67" s="177"/>
     </row>
     <row r="68" spans="7:24" x14ac:dyDescent="0.25">
       <c r="J68" s="97">
@@ -9033,7 +9024,7 @@
         <f t="shared" si="6"/>
         <v>-2.4615384615384595E-2</v>
       </c>
-      <c r="P68" s="173"/>
+      <c r="P68" s="177"/>
     </row>
     <row r="69" spans="7:24" x14ac:dyDescent="0.25">
       <c r="J69" s="97">
@@ -9055,7 +9046,7 @@
         <f t="shared" ref="N69:N132" si="15">(L69/L68)-1</f>
         <v>-2.8391167192429068E-2</v>
       </c>
-      <c r="P69" s="173"/>
+      <c r="P69" s="177"/>
     </row>
     <row r="70" spans="7:24" x14ac:dyDescent="0.25">
       <c r="J70" s="97">
@@ -9077,7 +9068,7 @@
         <f t="shared" si="15"/>
         <v>-2.5974025974025983E-2</v>
       </c>
-      <c r="P70" s="173"/>
+      <c r="P70" s="177"/>
     </row>
     <row r="71" spans="7:24" x14ac:dyDescent="0.25">
       <c r="J71" s="97">
@@ -9099,7 +9090,7 @@
         <f t="shared" si="15"/>
         <v>-3.0000000000000027E-2</v>
       </c>
-      <c r="P71" s="173"/>
+      <c r="P71" s="177"/>
     </row>
     <row r="72" spans="7:24" x14ac:dyDescent="0.25">
       <c r="J72" s="97">
@@ -9121,7 +9112,7 @@
         <f t="shared" si="15"/>
         <v>-2.7491408934707917E-2</v>
       </c>
-      <c r="P72" s="173"/>
+      <c r="P72" s="177"/>
       <c r="V72" t="s">
         <v>13</v>
       </c>
@@ -9150,7 +9141,7 @@
         <f t="shared" si="15"/>
         <v>-3.180212014134276E-2</v>
       </c>
-      <c r="P73" s="173"/>
+      <c r="P73" s="177"/>
       <c r="V73">
         <v>257</v>
       </c>
@@ -9181,7 +9172,7 @@
         <f t="shared" si="15"/>
         <v>-2.5547445255474477E-2</v>
       </c>
-      <c r="P74" s="173"/>
+      <c r="P74" s="177"/>
     </row>
     <row r="75" spans="7:24" x14ac:dyDescent="0.25">
       <c r="J75" s="97">
@@ -9203,7 +9194,7 @@
         <f t="shared" si="15"/>
         <v>-2.2471910112359605E-2</v>
       </c>
-      <c r="P75" s="173"/>
+      <c r="P75" s="177"/>
       <c r="V75">
         <v>300</v>
       </c>
@@ -9234,7 +9225,7 @@
         <f t="shared" si="15"/>
         <v>-2.6819923371647514E-2</v>
       </c>
-      <c r="P76" s="173"/>
+      <c r="P76" s="177"/>
     </row>
     <row r="77" spans="7:24" x14ac:dyDescent="0.25">
       <c r="J77" s="97">
@@ -9256,7 +9247,7 @@
         <f t="shared" si="15"/>
         <v>-2.7559055118110187E-2</v>
       </c>
-      <c r="P77" s="173"/>
+      <c r="P77" s="177"/>
     </row>
     <row r="78" spans="7:24" x14ac:dyDescent="0.25">
       <c r="G78" s="128" t="s">
@@ -9283,7 +9274,7 @@
         <f t="shared" si="15"/>
         <v>-2.4291497975708509E-2</v>
       </c>
-      <c r="P78" s="173"/>
+      <c r="P78" s="177"/>
     </row>
     <row r="79" spans="7:24" x14ac:dyDescent="0.25">
       <c r="J79" s="85">
@@ -9297,11 +9288,11 @@
         <f t="shared" si="13"/>
         <v>234</v>
       </c>
-      <c r="M79" s="174" t="str">
+      <c r="M79" s="167" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N79" s="175">
+      <c r="N79" s="168">
         <f t="shared" si="15"/>
         <v>-2.9045643153526979E-2</v>
       </c>
@@ -9319,11 +9310,11 @@
         <f t="shared" si="13"/>
         <v>227</v>
       </c>
-      <c r="M80" s="174" t="str">
+      <c r="M80" s="167" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N80" s="175">
+      <c r="N80" s="168">
         <f t="shared" si="15"/>
         <v>-2.9914529914529919E-2</v>
       </c>
@@ -9341,11 +9332,11 @@
         <f t="shared" si="13"/>
         <v>220</v>
       </c>
-      <c r="M81" s="174" t="str">
+      <c r="M81" s="167" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N81" s="175">
+      <c r="N81" s="168">
         <f t="shared" si="15"/>
         <v>-3.0837004405286361E-2</v>
       </c>
@@ -9363,11 +9354,11 @@
         <f t="shared" si="13"/>
         <v>214</v>
       </c>
-      <c r="M82" s="174" t="str">
+      <c r="M82" s="167" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N82" s="175">
+      <c r="N82" s="168">
         <f t="shared" si="15"/>
         <v>-2.7272727272727226E-2</v>
       </c>
@@ -9407,11 +9398,11 @@
         <f t="shared" si="13"/>
         <v>202</v>
       </c>
-      <c r="M84" s="174" t="str">
+      <c r="M84" s="167" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N84" s="175">
+      <c r="N84" s="168">
         <f t="shared" si="15"/>
         <v>-2.4154589371980673E-2</v>
       </c>
@@ -9428,11 +9419,11 @@
         <f t="shared" si="13"/>
         <v>197</v>
       </c>
-      <c r="M85" s="174" t="str">
+      <c r="M85" s="167" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N85" s="175">
+      <c r="N85" s="168">
         <f t="shared" si="15"/>
         <v>-2.4752475247524774E-2</v>
       </c>
@@ -9449,11 +9440,11 @@
         <f t="shared" si="13"/>
         <v>191</v>
       </c>
-      <c r="M86" s="174" t="str">
+      <c r="M86" s="167" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N86" s="175">
+      <c r="N86" s="168">
         <f t="shared" si="15"/>
         <v>-3.0456852791878153E-2</v>
       </c>
@@ -9470,11 +9461,11 @@
         <f t="shared" si="13"/>
         <v>186</v>
       </c>
-      <c r="M87" s="174" t="str">
+      <c r="M87" s="167" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N87" s="175">
+      <c r="N87" s="168">
         <f t="shared" si="15"/>
         <v>-2.6178010471204161E-2</v>
       </c>
@@ -9491,40 +9482,38 @@
         <f t="shared" si="13"/>
         <v>181</v>
       </c>
-      <c r="M88" s="174" t="str">
+      <c r="M88" s="167" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N88" s="175">
+      <c r="N88" s="168">
         <f t="shared" si="15"/>
         <v>-2.6881720430107503E-2</v>
       </c>
     </row>
     <row r="89" spans="6:16" x14ac:dyDescent="0.25">
-      <c r="F89" s="180"/>
-      <c r="G89" s="181" t="s">
+      <c r="F89" s="137"/>
+      <c r="G89" s="170"/>
+      <c r="H89" s="170" t="s">
         <v>100</v>
       </c>
-      <c r="H89" s="182" t="s">
-        <v>18</v>
-      </c>
-      <c r="I89" s="137"/>
-      <c r="J89" s="176">
+      <c r="I89" s="169"/>
+      <c r="J89" s="178">
         <v>66</v>
       </c>
-      <c r="K89" s="177">
+      <c r="K89" s="179">
         <f t="shared" si="17"/>
         <v>175.80000000000007</v>
       </c>
-      <c r="L89" s="177">
+      <c r="L89" s="179">
         <f t="shared" si="13"/>
         <v>176</v>
       </c>
-      <c r="M89" s="178" t="str">
+      <c r="M89" s="180" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N89" s="179">
+      <c r="N89" s="181">
         <f t="shared" si="15"/>
         <v>-2.7624309392265234E-2</v>
       </c>
@@ -9541,11 +9530,11 @@
         <f t="shared" si="13"/>
         <v>171</v>
       </c>
-      <c r="M90" s="174" t="str">
+      <c r="M90" s="167" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N90" s="175">
+      <c r="N90" s="168">
         <f t="shared" si="15"/>
         <v>-2.8409090909090939E-2</v>
       </c>
@@ -9562,11 +9551,11 @@
         <f t="shared" si="13"/>
         <v>165</v>
       </c>
-      <c r="M91" s="174" t="str">
+      <c r="M91" s="167" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N91" s="175">
+      <c r="N91" s="168">
         <f t="shared" si="15"/>
         <v>-3.5087719298245612E-2</v>
       </c>
@@ -9583,11 +9572,11 @@
         <f t="shared" si="13"/>
         <v>160</v>
       </c>
-      <c r="M92" s="174" t="str">
+      <c r="M92" s="167" t="str">
         <f t="shared" si="14"/>
         <v>OK</v>
       </c>
-      <c r="N92" s="175">
+      <c r="N92" s="168">
         <f t="shared" si="15"/>
         <v>-3.0303030303030276E-2</v>
       </c>

</xml_diff>